<commit_message>
Data Source List.  Added a "Query" column to the Excel file in the Data Source List to identify data sources using SQL Query in the Qlik Compose Mappings definition.
</commit_message>
<xml_diff>
--- a/Documentations/Data_Source_List_EN_v3.3.xlsx
+++ b/Documentations/Data_Source_List_EN_v3.3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://qliktechnologies365-my.sharepoint.com/personal/amo_qlik_com/Documents/04_Qlik Replicate/Accelerator/ODP作業/SAP Acceleratorバージョン管理/20231215_文書/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://qliktechnologies365-my.sharepoint.com/personal/amo_qlik_com/Documents/Documents/GitHub/Qlik_SAP_Accelerators_For_QDI/Documentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{AA4868D6-6CCF-4F24-9F5F-C426523F1864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93B1B205-2D27-4E52-B0B1-2F8FA8C156D0}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{AA4868D6-6CCF-4F24-9F5F-C426523F1864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FB16155-C156-4BC9-A56E-CD43506BB779}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="210" windowWidth="25440" windowHeight="15270" activeTab="4" xr2:uid="{35D0DF68-4C88-4D71-9D2B-AF545C1DDC9A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{35D0DF68-4C88-4D71-9D2B-AF545C1DDC9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Order to Cash" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,10 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">All!$A$1:$H$88</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Finance!$A$1:$I$38</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Inventory!$A$1:$I$31</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Order to Cash'!$A$1:$I$32</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Procurement!$A$1:$I$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Finance!$A$1:$K$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Inventory!$A$1:$J$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Order to Cash'!$A$1:$J$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Procurement!$A$1:$J$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="392">
   <si>
     <t>Full / Delta</t>
   </si>
@@ -1386,6 +1386,9 @@
   </si>
   <si>
     <t>Hierarchy</t>
+  </si>
+  <si>
+    <t>Query</t>
   </si>
 </sst>
 </file>
@@ -1640,9 +1643,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1680,7 +1683,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1786,7 +1789,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1928,7 +1931,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1936,10 +1939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA63AFC-DEA2-4600-8592-D582621CDE75}">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1954,7 +1957,7 @@
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="20" t="s">
         <v>205</v>
       </c>
@@ -1982,8 +1985,11 @@
       <c r="I1" s="20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="20" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -2009,8 +2015,9 @@
       <c r="I2" s="16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="16"/>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -2034,8 +2041,11 @@
         <v>36</v>
       </c>
       <c r="I3" s="16"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -2059,8 +2069,11 @@
         <v>36</v>
       </c>
       <c r="I4" s="16"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -2086,8 +2099,9 @@
       <c r="I5" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="17"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -2113,8 +2127,9 @@
       <c r="I6" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="17"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -2140,8 +2155,9 @@
       <c r="I7" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" s="17"/>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -2167,8 +2183,9 @@
       <c r="I8" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="17"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -2194,8 +2211,11 @@
       <c r="I9" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="15">
         <v>9</v>
       </c>
@@ -2219,8 +2239,11 @@
         <v>36</v>
       </c>
       <c r="I10" s="17"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -2244,8 +2267,11 @@
         <v>36</v>
       </c>
       <c r="I11" s="17"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -2269,8 +2295,9 @@
         <v>36</v>
       </c>
       <c r="I12" s="17"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="17"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -2296,8 +2323,9 @@
       <c r="I13" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="17"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -2323,8 +2351,9 @@
       <c r="I14" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -2350,8 +2379,9 @@
       <c r="I15" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" s="17"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="15">
         <v>15</v>
       </c>
@@ -2377,8 +2407,9 @@
       <c r="I16" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" s="17"/>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -2404,8 +2435,9 @@
       <c r="I17" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="17"/>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -2431,8 +2463,9 @@
       <c r="I18" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" s="17"/>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -2458,8 +2491,9 @@
       <c r="I19" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1">
+      <c r="J19" s="17"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" customHeight="1">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -2485,8 +2519,9 @@
       <c r="I20" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" s="17"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -2512,8 +2547,9 @@
       <c r="I21" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" s="17"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -2539,8 +2575,9 @@
       <c r="I22" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" s="17"/>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -2566,8 +2603,9 @@
       <c r="I23" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" s="17"/>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -2593,8 +2631,9 @@
       <c r="I24" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" s="17"/>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -2620,8 +2659,9 @@
       <c r="I25" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" s="17"/>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -2647,8 +2687,9 @@
       <c r="I26" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" s="17"/>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -2672,8 +2713,11 @@
         <v>36</v>
       </c>
       <c r="I27" s="17"/>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -2697,8 +2741,11 @@
         <v>36</v>
       </c>
       <c r="I28" s="17"/>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -2722,8 +2769,11 @@
         <v>36</v>
       </c>
       <c r="I29" s="17"/>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -2747,8 +2797,11 @@
         <v>36</v>
       </c>
       <c r="I30" s="17"/>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -2772,8 +2825,11 @@
         <v>36</v>
       </c>
       <c r="I31" s="17"/>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="J31" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -2797,8 +2853,11 @@
         <v>36</v>
       </c>
       <c r="I32" s="17"/>
-    </row>
-    <row r="33" spans="1:9" s="2" customFormat="1">
+      <c r="J32" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="2" customFormat="1">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -2822,8 +2881,9 @@
         <v>36</v>
       </c>
       <c r="I33" s="17"/>
-    </row>
-    <row r="34" spans="1:9" s="2" customFormat="1">
+      <c r="J33" s="17"/>
+    </row>
+    <row r="34" spans="1:10" s="2" customFormat="1">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -2845,8 +2905,9 @@
         <v>36</v>
       </c>
       <c r="I34" s="17"/>
-    </row>
-    <row r="35" spans="1:9" s="2" customFormat="1">
+      <c r="J34" s="17"/>
+    </row>
+    <row r="35" spans="1:10" s="2" customFormat="1">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
@@ -2856,8 +2917,9 @@
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
-    </row>
-    <row r="36" spans="1:9" s="2" customFormat="1">
+      <c r="J35" s="13"/>
+    </row>
+    <row r="36" spans="1:10" s="2" customFormat="1">
       <c r="A36" s="2" t="s">
         <v>306</v>
       </c>
@@ -2865,7 +2927,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="2" customFormat="1">
+    <row r="37" spans="1:10" s="2" customFormat="1">
       <c r="A37" s="2" t="s">
         <v>308</v>
       </c>
@@ -2873,7 +2935,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="2" customFormat="1">
+    <row r="38" spans="1:10" s="2" customFormat="1">
       <c r="A38" s="2" t="s">
         <v>4</v>
       </c>
@@ -2881,7 +2943,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="2" customFormat="1">
+    <row r="39" spans="1:10" s="2" customFormat="1">
       <c r="A39" s="2" t="s">
         <v>311</v>
       </c>
@@ -2889,7 +2951,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="2" customFormat="1">
+    <row r="40" spans="1:10" s="2" customFormat="1">
       <c r="A40" s="2" t="s">
         <v>313</v>
       </c>
@@ -2897,7 +2959,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="2" customFormat="1">
+    <row r="41" spans="1:10" s="2" customFormat="1">
       <c r="A41" s="2" t="s">
         <v>305</v>
       </c>
@@ -2905,7 +2967,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="2" customFormat="1">
+    <row r="42" spans="1:10" s="2" customFormat="1">
       <c r="A42" s="2" t="s">
         <v>33</v>
       </c>
@@ -2913,7 +2975,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="2" customFormat="1">
+    <row r="43" spans="1:10" s="2" customFormat="1">
       <c r="A43" s="2" t="s">
         <v>316</v>
       </c>
@@ -2921,7 +2983,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="2" customFormat="1">
+    <row r="44" spans="1:10" s="2" customFormat="1">
       <c r="A44" s="2" t="s">
         <v>318</v>
       </c>
@@ -2929,7 +2991,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="2" customFormat="1">
+    <row r="45" spans="1:10" s="2" customFormat="1">
       <c r="A45" s="2" t="s">
         <v>320</v>
       </c>
@@ -2937,7 +2999,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="2" customFormat="1">
+    <row r="46" spans="1:10" s="2" customFormat="1">
       <c r="A46" s="2" t="s">
         <v>322</v>
       </c>
@@ -2945,7 +3007,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="2" customFormat="1">
+    <row r="47" spans="1:10" s="2" customFormat="1">
       <c r="A47" s="2" t="s">
         <v>324</v>
       </c>
@@ -2953,7 +3015,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="2" customFormat="1">
+    <row r="48" spans="1:10" s="2" customFormat="1">
       <c r="A48" s="2" t="s">
         <v>326</v>
       </c>
@@ -2994,11 +3056,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I32" xr:uid="{6CA63AFC-DEA2-4600-8592-D582621CDE75}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I35">
-      <sortCondition ref="E1:E32"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:J34" xr:uid="{6CA63AFC-DEA2-4600-8592-D582621CDE75}"/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3007,10 +3065,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2CFF8A4-B7BC-43A6-8B98-38E2623B1AA7}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.28515625" defaultRowHeight="14.25"/>
@@ -3023,11 +3081,11 @@
     <col min="6" max="6" width="13.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="21.28515625" style="2"/>
+    <col min="9" max="10" width="8.42578125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="21.28515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="20" t="s">
         <v>205</v>
       </c>
@@ -3055,8 +3113,11 @@
       <c r="I1" s="20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="14" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -3080,8 +3141,9 @@
         <v>36</v>
       </c>
       <c r="I2" s="15"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -3107,8 +3169,11 @@
       <c r="I3" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -3132,8 +3197,9 @@
         <v>36</v>
       </c>
       <c r="I4" s="15"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="15"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -3157,8 +3223,9 @@
         <v>36</v>
       </c>
       <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -3182,8 +3249,11 @@
         <v>36</v>
       </c>
       <c r="I6" s="15"/>
-    </row>
-    <row r="7" spans="1:9" ht="18.75" customHeight="1">
+      <c r="J6" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" customHeight="1">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -3209,8 +3279,9 @@
       <c r="I7" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1">
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="1:10" ht="17.25" customHeight="1">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -3236,8 +3307,11 @@
       <c r="I8" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -3261,8 +3335,9 @@
         <v>36</v>
       </c>
       <c r="I9" s="15"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" s="15"/>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="15">
         <v>9</v>
       </c>
@@ -3286,8 +3361,11 @@
         <v>36</v>
       </c>
       <c r="I10" s="15"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -3311,8 +3389,9 @@
         <v>36</v>
       </c>
       <c r="I11" s="15"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" s="15"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -3338,8 +3417,9 @@
       <c r="I12" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="15"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -3365,8 +3445,9 @@
       <c r="I13" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="15"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3392,8 +3473,9 @@
       <c r="I14" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -3419,8 +3501,9 @@
       <c r="I15" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" s="15"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="15">
         <v>15</v>
       </c>
@@ -3446,8 +3529,11 @@
       <c r="I16" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -3471,8 +3557,9 @@
         <v>36</v>
       </c>
       <c r="I17" s="15"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -3496,8 +3583,9 @@
         <v>36</v>
       </c>
       <c r="I18" s="15"/>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -3521,8 +3609,9 @@
         <v>36</v>
       </c>
       <c r="I19" s="15"/>
-    </row>
-    <row r="20" spans="1:9" ht="17.25" customHeight="1">
+      <c r="J19" s="15"/>
+    </row>
+    <row r="20" spans="1:10" ht="17.25" customHeight="1">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -3548,8 +3637,9 @@
       <c r="I20" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" s="15"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -3573,8 +3663,9 @@
         <v>36</v>
       </c>
       <c r="I21" s="15"/>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" s="15"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -3600,8 +3691,9 @@
       <c r="I22" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" s="15"/>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -3625,8 +3717,11 @@
         <v>36</v>
       </c>
       <c r="I23" s="15"/>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -3650,8 +3745,11 @@
         <v>36</v>
       </c>
       <c r="I24" s="15"/>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -3675,8 +3773,11 @@
         <v>36</v>
       </c>
       <c r="I25" s="15"/>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -3700,8 +3801,11 @@
         <v>36</v>
       </c>
       <c r="I26" s="15"/>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -3725,8 +3829,9 @@
         <v>36</v>
       </c>
       <c r="I27" s="15"/>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" s="15"/>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -3752,8 +3857,9 @@
       <c r="I28" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="J28" s="15"/>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -3779,8 +3885,9 @@
       <c r="I29" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" s="15"/>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -3804,8 +3911,11 @@
         <v>36</v>
       </c>
       <c r="I30" s="15"/>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="J30" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -3827,6 +3937,7 @@
         <v>36</v>
       </c>
       <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2" t="s">
@@ -3965,11 +4076,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I31" xr:uid="{E2CFF8A4-B7BC-43A6-8B98-38E2623B1AA7}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I31">
-      <sortCondition ref="E1:E31"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:J31" xr:uid="{E2CFF8A4-B7BC-43A6-8B98-38E2623B1AA7}"/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3978,10 +4085,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE96B8FB-2046-4612-B3AC-21580330EA1F}">
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -3998,7 +4105,7 @@
     <col min="11" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="27" customHeight="1">
+    <row r="1" spans="1:11" ht="27" customHeight="1">
       <c r="A1" s="20" t="s">
         <v>205</v>
       </c>
@@ -4029,8 +4136,11 @@
       <c r="J1" s="14" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="14" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -4055,8 +4165,11 @@
       </c>
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -4085,8 +4198,9 @@
       <c r="J3" s="16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -4113,8 +4227,11 @@
       <c r="J4" s="16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -4139,8 +4256,9 @@
       </c>
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5" s="16"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -4167,8 +4285,9 @@
         <v>36</v>
       </c>
       <c r="J6" s="15"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6" s="16"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -4193,8 +4312,11 @@
       </c>
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -4219,8 +4341,9 @@
       </c>
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="16"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -4245,8 +4368,9 @@
       </c>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" s="16"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="15">
         <v>9</v>
       </c>
@@ -4271,8 +4395,11 @@
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -4297,8 +4424,9 @@
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" s="16"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -4323,8 +4451,9 @@
       </c>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12" s="16"/>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -4349,8 +4478,9 @@
       </c>
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13" s="16"/>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -4375,8 +4505,11 @@
       </c>
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -4401,8 +4534,9 @@
       </c>
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15" s="16"/>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="15">
         <v>15</v>
       </c>
@@ -4429,8 +4563,11 @@
         <v>36</v>
       </c>
       <c r="J16" s="16"/>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16" s="16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -4457,8 +4594,9 @@
         <v>36</v>
       </c>
       <c r="J17" s="16"/>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17" s="16"/>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -4483,8 +4621,11 @@
       </c>
       <c r="I18" s="15"/>
       <c r="J18" s="16"/>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18" s="16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -4511,8 +4652,9 @@
         <v>36</v>
       </c>
       <c r="J19" s="16"/>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19" s="16"/>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -4539,8 +4681,9 @@
         <v>36</v>
       </c>
       <c r="J20" s="16"/>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20" s="16"/>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -4565,8 +4708,11 @@
       </c>
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21" s="16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -4595,8 +4741,9 @@
       <c r="J22" s="16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22" s="16"/>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -4625,8 +4772,9 @@
       <c r="J23" s="16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23" s="16"/>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -4653,8 +4801,9 @@
         <v>36</v>
       </c>
       <c r="J24" s="16"/>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24" s="16"/>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -4681,8 +4830,9 @@
         <v>36</v>
       </c>
       <c r="J25" s="16"/>
-    </row>
-    <row r="26" spans="1:10" ht="17.25" customHeight="1">
+      <c r="K25" s="16"/>
+    </row>
+    <row r="26" spans="1:11" ht="17.25" customHeight="1">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -4709,8 +4859,9 @@
         <v>36</v>
       </c>
       <c r="J26" s="16"/>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26" s="16"/>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -4737,8 +4888,9 @@
         <v>36</v>
       </c>
       <c r="J27" s="16"/>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27" s="16"/>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -4765,8 +4917,9 @@
         <v>36</v>
       </c>
       <c r="J28" s="16"/>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="K28" s="16"/>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -4793,8 +4946,9 @@
         <v>36</v>
       </c>
       <c r="J29" s="16"/>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29" s="16"/>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -4819,8 +4973,11 @@
       </c>
       <c r="I30" s="16"/>
       <c r="J30" s="16"/>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="K30" s="16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -4847,8 +5004,9 @@
         <v>36</v>
       </c>
       <c r="J31" s="16"/>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="K31" s="16"/>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -4875,8 +5033,11 @@
         <v>36</v>
       </c>
       <c r="J32" s="16"/>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="K32" s="16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -4901,8 +5062,9 @@
       </c>
       <c r="I33" s="16"/>
       <c r="J33" s="16"/>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="K33" s="16"/>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -4927,8 +5089,11 @@
       </c>
       <c r="I34" s="16"/>
       <c r="J34" s="16"/>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="K34" s="16" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -4955,8 +5120,9 @@
         <v>36</v>
       </c>
       <c r="J35" s="16"/>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="K35" s="16"/>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -4983,8 +5149,9 @@
         <v>36</v>
       </c>
       <c r="J36" s="16"/>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="K36" s="16"/>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -5009,8 +5176,9 @@
         <v>36</v>
       </c>
       <c r="J37" s="16"/>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="K37" s="16"/>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -5033,8 +5201,9 @@
       </c>
       <c r="I38" s="16"/>
       <c r="J38" s="16"/>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="K38" s="16"/>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -5057,8 +5226,9 @@
       </c>
       <c r="I39" s="16"/>
       <c r="J39" s="16"/>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="K39" s="16"/>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -5081,8 +5251,9 @@
       </c>
       <c r="I40" s="16"/>
       <c r="J40" s="16"/>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="K40" s="16"/>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -5105,8 +5276,9 @@
       </c>
       <c r="I41" s="16"/>
       <c r="J41" s="16"/>
-    </row>
-    <row r="42" spans="1:10">
+      <c r="K41" s="16"/>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="11"/>
@@ -5117,8 +5289,9 @@
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
-    </row>
-    <row r="44" spans="1:10">
+      <c r="K42" s="13"/>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" s="2" t="s">
         <v>306</v>
       </c>
@@ -5126,7 +5299,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:11">
       <c r="A45" s="2" t="s">
         <v>308</v>
       </c>
@@ -5134,7 +5307,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:11">
       <c r="A46" s="2" t="s">
         <v>4</v>
       </c>
@@ -5142,7 +5315,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:11">
       <c r="A47" s="2" t="s">
         <v>311</v>
       </c>
@@ -5150,7 +5323,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:11">
       <c r="A48" s="2" t="s">
         <v>313</v>
       </c>
@@ -5290,11 +5463,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I38" xr:uid="{6CA63AFC-DEA2-4600-8592-D582621CDE75}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I38">
-      <sortCondition ref="B1:B38"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:K41" xr:uid="{FE96B8FB-2046-4612-B3AC-21580330EA1F}"/>
   <phoneticPr fontId="1"/>
   <hyperlinks>
     <hyperlink ref="A68" r:id="rId1" xr:uid="{5C2F3883-8135-4C59-BC0E-A8B8FEE4B90F}"/>
@@ -5306,10 +5475,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE1BC69-ED35-49BA-85D5-1C8C38BE75C7}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -5322,13 +5491,12 @@
     <col min="6" max="6" width="13.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" style="4" customWidth="1"/>
+    <col min="9" max="10" width="8.42578125" style="2" customWidth="1"/>
     <col min="11" max="11" width="9" style="4" customWidth="1"/>
     <col min="12" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="20" t="s">
         <v>205</v>
       </c>
@@ -5356,8 +5524,11 @@
       <c r="I1" s="20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="14" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -5381,8 +5552,11 @@
         <v>36</v>
       </c>
       <c r="I2" s="15"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -5406,8 +5580,9 @@
         <v>36</v>
       </c>
       <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3" s="15"/>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -5431,8 +5606,9 @@
         <v>36</v>
       </c>
       <c r="I4" s="15"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" s="15"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -5456,8 +5632,9 @@
         <v>36</v>
       </c>
       <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -5483,8 +5660,11 @@
       <c r="I6" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -5510,8 +5690,9 @@
       <c r="I7" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -5537,8 +5718,9 @@
       <c r="I8" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -5564,8 +5746,11 @@
       <c r="I9" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="15">
         <v>9</v>
       </c>
@@ -5589,8 +5774,11 @@
         <v>36</v>
       </c>
       <c r="I10" s="15"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -5614,8 +5802,11 @@
         <v>36</v>
       </c>
       <c r="I11" s="15"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -5639,8 +5830,11 @@
         <v>36</v>
       </c>
       <c r="I12" s="15"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -5664,8 +5858,9 @@
         <v>36</v>
       </c>
       <c r="I13" s="15"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13" s="15"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -5689,8 +5884,9 @@
         <v>36</v>
       </c>
       <c r="I14" s="15"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -5716,8 +5912,9 @@
       <c r="I15" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15" s="15"/>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="15">
         <v>15</v>
       </c>
@@ -5743,8 +5940,9 @@
       <c r="I16" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -5768,8 +5966,9 @@
         <v>36</v>
       </c>
       <c r="I17" s="15"/>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -5793,8 +5992,9 @@
         <v>36</v>
       </c>
       <c r="I18" s="15"/>
-    </row>
-    <row r="19" spans="1:9">
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -5820,8 +6020,9 @@
       <c r="I19" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
+      <c r="J19" s="15"/>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -5847,8 +6048,9 @@
       <c r="I20" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
+      <c r="J20" s="15"/>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -5874,8 +6076,9 @@
       <c r="I21" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21" s="15"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -5901,8 +6104,9 @@
       <c r="I22" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="J22" s="15"/>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -5928,8 +6132,9 @@
       <c r="I23" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" s="15"/>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -5955,8 +6160,9 @@
       <c r="I24" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="J24" s="15"/>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -5982,8 +6188,9 @@
       <c r="I25" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="J25" s="15"/>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -6009,8 +6216,9 @@
       <c r="I26" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="J26" s="15"/>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -6036,8 +6244,9 @@
       <c r="I27" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
+      <c r="J27" s="15"/>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -6059,8 +6268,9 @@
         <v>36</v>
       </c>
       <c r="I28" s="15"/>
-    </row>
-    <row r="29" spans="1:9" ht="24">
+      <c r="J28" s="15"/>
+    </row>
+    <row r="29" spans="1:10" ht="24">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -6082,8 +6292,9 @@
         <v>36</v>
       </c>
       <c r="I29" s="15"/>
-    </row>
-    <row r="30" spans="1:9">
+      <c r="J29" s="15"/>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -6105,8 +6316,9 @@
         <v>36</v>
       </c>
       <c r="I30" s="15"/>
-    </row>
-    <row r="32" spans="1:9" s="2" customFormat="1" ht="14.25">
+      <c r="J30" s="15"/>
+    </row>
+    <row r="32" spans="1:10" s="2" customFormat="1" ht="14.25">
       <c r="A32" s="2" t="s">
         <v>306</v>
       </c>
@@ -6243,7 +6455,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I30" xr:uid="{FCE1BC69-ED35-49BA-85D5-1C8C38BE75C7}"/>
+  <autoFilter ref="A1:J30" xr:uid="{FCE1BC69-ED35-49BA-85D5-1C8C38BE75C7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I30">
     <sortCondition ref="B2:B30"/>
   </sortState>
@@ -6257,7 +6469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344D9DAD-F9DB-49D3-8BB6-56B5B644B394}">
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>